<commit_message>
Best Lifter page from selection
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionBook/Masters-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionBook/Masters-A4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B79721-88AB-4691-8F36-3C2CD6FEB6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979987EC-A17A-4EE6-BF90-D5875C546F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25920" yWindow="2745" windowWidth="24225" windowHeight="11295" tabRatio="555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="33" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="6">WSMF!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">WT!$10:$10</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="155">
   <si>
     <t>M/F</t>
   </si>
@@ -489,6 +489,33 @@
   </si>
   <si>
     <t>${l.qAge}</t>
+  </si>
+  <si>
+    <t>${t.get("Medal.Gold")}</t>
+  </si>
+  <si>
+    <t>${t.get("Medal.Silver")}</t>
+  </si>
+  <si>
+    <t>${t.get("Medal.Bronze")}</t>
+  </si>
+  <si>
+    <t>$[sumif(a10:a14,a5,n10:n14)]</t>
+  </si>
+  <si>
+    <t>$[sumif(a10:a14,a5,o10:o14)]</t>
+  </si>
+  <si>
+    <t>$[sumif(a10:a14,a5,p10:p14)]</t>
+  </si>
+  <si>
+    <t>$[countif(j12:j12,1)]</t>
+  </si>
+  <si>
+    <t>$[countif(j12:j12,2)]</t>
+  </si>
+  <si>
+    <t>$[countif(j12:j12,3)]</t>
   </si>
 </sst>
 </file>
@@ -668,7 +695,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1075,6 +1102,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1089,7 +1157,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1354,10 +1422,44 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1377,32 +1479,29 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1425,30 +1524,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1988,14 +2063,14 @@
       <c r="A1" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
       <c r="J1" s="53" t="s">
@@ -2009,14 +2084,14 @@
       <c r="A2" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
       <c r="H2" s="53"/>
       <c r="I2" s="53"/>
       <c r="J2" s="53" t="s">
@@ -2030,14 +2105,14 @@
       <c r="A3" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="53"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -5568,7 +5643,7 @@
   <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G2"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5597,58 +5672,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="102" t="s">
+      <c r="D1" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="104" t="s">
+      <c r="I1" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="105" t="s">
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="112" t="s">
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="112"/>
+      <c r="T1" s="110"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
       <c r="I2" s="38">
         <v>1</v>
       </c>
@@ -5806,11 +5881,11 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
-      <c r="R12" s="101"/>
+      <c r="R12" s="111"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
-      <c r="R13" s="101"/>
+      <c r="R13" s="111"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
@@ -6088,11 +6163,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="S1:T1"/>
     <mergeCell ref="R12:R13"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
@@ -6100,6 +6170,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:R1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5">
     <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
@@ -6124,572 +6199,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FABBA97-39C6-49D5-A158-F8A84417C014}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:W102"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="12" width="7.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="22" customWidth="1"/>
-    <col min="15" max="17" width="7.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" style="22" customWidth="1"/>
-    <col min="21" max="22" width="10.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="119" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="119" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="121" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="102" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="124" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="113" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="114" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="116" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="117" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="104" t="s">
-        <v>142</v>
-      </c>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
-      <c r="V1"/>
-      <c r="W1"/>
-    </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="12">
-        <v>1</v>
-      </c>
-      <c r="J2" s="12">
-        <v>2</v>
-      </c>
-      <c r="K2" s="12">
-        <v>3</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="12">
-        <v>1</v>
-      </c>
-      <c r="N2" s="12">
-        <v>2</v>
-      </c>
-      <c r="O2" s="12">
-        <v>3</v>
-      </c>
-      <c r="P2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="S2" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="T2" s="50" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-    </row>
-    <row r="4" spans="1:23" s="5" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" s="64" t="s">
-        <v>144</v>
-      </c>
-      <c r="S4" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="T4" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C10" s="1"/>
-      <c r="R10" s="101"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
-      <c r="R11" s="101"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C71" s="1"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C96" s="1"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C97" s="1"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C98" s="1"/>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C100" s="1"/>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C101" s="1"/>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C102" s="1"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="13">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:T1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B4:C4">
-    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
-      <formula>AND(("$'Hommes Sinclair'.$#REF!$#REF!"),"$'Hommes Sinclair'.$#REF!$#REF!","$'Hommes Sinclair'.$#REF!$#REF!")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{CC0A5D4E-226B-4BC3-B392-FD2BD37BEA1D}">
-      <formula1>0</formula1>
-      <formula2>200</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="75" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
-    <oddFooter>&amp;R&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6722,62 +6231,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="117" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="102" t="s">
+      <c r="D1" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="124" t="s">
+      <c r="F1" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="114" t="s">
+      <c r="H1" s="123" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116" t="s">
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="117" t="s">
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="104" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
+      <c r="R1" s="114" t="s">
+        <v>142</v>
+      </c>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
       <c r="V1"/>
       <c r="W1"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="115"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="124"/>
       <c r="I2" s="12">
         <v>1</v>
       </c>
@@ -6802,12 +6311,12 @@
       <c r="P2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="118"/>
+      <c r="Q2" s="127"/>
       <c r="R2" s="49" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="S2" s="39" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="T2" s="50" t="s">
         <v>80</v>
@@ -6887,10 +6396,10 @@
         <v>20</v>
       </c>
       <c r="R4" s="64" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
       <c r="S4" s="65" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="T4" s="66" t="s">
         <v>48</v>
@@ -6937,11 +6446,11 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
-      <c r="R10" s="101"/>
+      <c r="R10" s="111"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
-      <c r="R11" s="101"/>
+      <c r="R11" s="111"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
@@ -7219,11 +6728,572 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B4:C4">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+      <formula>AND(("$'Hommes Sinclair'.$#REF!$#REF!"),"$'Hommes Sinclair'.$#REF!$#REF!","$'Hommes Sinclair'.$#REF!$#REF!")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{CC0A5D4E-226B-4BC3-B392-FD2BD37BEA1D}">
+      <formula1>0</formula1>
+      <formula2>200</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
+  <pageSetup paperSize="9" scale="75" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
+    <oddFooter>&amp;R&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:W102"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="12" width="7.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" style="22" customWidth="1"/>
+    <col min="15" max="17" width="7.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" style="22" customWidth="1"/>
+    <col min="21" max="22" width="10.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="117" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="117" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="119" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="112" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="116" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="122" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="123" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="125" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="126" t="s">
+        <v>78</v>
+      </c>
+      <c r="R1" s="114" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="V1"/>
+      <c r="W1"/>
+    </row>
+    <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="12">
+        <v>1</v>
+      </c>
+      <c r="J2" s="12">
+        <v>2</v>
+      </c>
+      <c r="K2" s="12">
+        <v>3</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="12">
+        <v>1</v>
+      </c>
+      <c r="N2" s="12">
+        <v>2</v>
+      </c>
+      <c r="O2" s="12">
+        <v>3</v>
+      </c>
+      <c r="P2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" s="50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="1:23" s="5" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C10" s="1"/>
+      <c r="R10" s="111"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+      <c r="R11" s="111"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C102" s="1"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="13">
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="R10:R11"/>
     <mergeCell ref="G1:G2"/>
@@ -7232,6 +7302,11 @@
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:T1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C4">
     <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
@@ -7290,58 +7365,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="102" t="s">
+      <c r="D1" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="104" t="s">
+      <c r="I1" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="105" t="s">
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="112" t="s">
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="112"/>
+      <c r="T1" s="110"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
       <c r="I2" s="38">
         <v>1</v>
       </c>
@@ -7500,11 +7575,11 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
-      <c r="R12" s="101"/>
+      <c r="R12" s="111"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
-      <c r="R13" s="101"/>
+      <c r="R13" s="111"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
@@ -7782,11 +7857,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="N1:R1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="R12:R13"/>
     <mergeCell ref="E1:E2"/>
@@ -7794,6 +7864,11 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:M1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5">
     <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
@@ -7849,62 +7924,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="117" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="102" t="s">
+      <c r="D1" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="124" t="s">
+      <c r="F1" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="114" t="s">
+      <c r="H1" s="123" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116" t="s">
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="117" t="s">
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="104" t="s">
+      <c r="R1" s="114" t="s">
         <v>142</v>
       </c>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
       <c r="V1"/>
       <c r="W1"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="115"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="124"/>
       <c r="I2" s="12">
         <v>1</v>
       </c>
@@ -7929,7 +8004,7 @@
       <c r="P2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="118"/>
+      <c r="Q2" s="127"/>
       <c r="R2" s="49" t="s">
         <v>143</v>
       </c>
@@ -8063,11 +8138,11 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
-      <c r="R10" s="101"/>
+      <c r="R10" s="111"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
-      <c r="R11" s="101"/>
+      <c r="R11" s="111"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
@@ -8330,12 +8405,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="R10:R11"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
@@ -8343,6 +8412,12 @@
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:T1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C4">
     <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
@@ -8373,7 +8448,7 @@
   <dimension ref="A1:W97"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8398,62 +8473,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="117" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="102" t="s">
+      <c r="D1" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="124" t="s">
+      <c r="F1" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="114" t="s">
+      <c r="H1" s="123" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116" t="s">
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="117" t="s">
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="104" t="s">
+      <c r="R1" s="114" t="s">
         <v>81</v>
       </c>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
       <c r="V1"/>
       <c r="W1"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="115"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="124"/>
       <c r="I2" s="12">
         <v>1</v>
       </c>
@@ -8478,7 +8553,7 @@
       <c r="P2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="118"/>
+      <c r="Q2" s="127"/>
       <c r="R2" s="49" t="s">
         <v>81</v>
       </c>
@@ -8878,11 +8953,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="F1:F2"/>
@@ -8890,6 +8960,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:P1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C4">
     <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
@@ -8946,7 +9021,10 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M2"/>
+      <c r="P2"/>
+    </row>
     <row r="3" spans="1:19" s="10" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>74</v>
@@ -8960,6 +9038,18 @@
       <c r="D3" s="44" t="s">
         <v>66</v>
       </c>
+      <c r="M3" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="O3" s="99" t="s">
+        <v>147</v>
+      </c>
+      <c r="P3" s="99" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -8967,8 +9057,8 @@
       </c>
       <c r="B4" s="20"/>
       <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4"/>
@@ -8986,6 +9076,18 @@
       </c>
       <c r="D5" s="42" t="s">
         <v>44</v>
+      </c>
+      <c r="M5" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="O5" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="P5" s="100" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -9054,6 +9156,15 @@
       <c r="M10" s="40" t="s">
         <v>86</v>
       </c>
+      <c r="N10" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="O10" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="P10" s="99" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -9104,8 +9215,17 @@
       <c r="L12" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="101" t="s">
         <v>36</v>
+      </c>
+      <c r="N12" s="101" t="s">
+        <v>152</v>
+      </c>
+      <c r="O12" s="101" t="s">
+        <v>153</v>
+      </c>
+      <c r="P12" s="101" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -9113,6 +9233,9 @@
         <v>22</v>
       </c>
       <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
@@ -9134,6 +9257,9 @@
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -9170,7 +9296,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="81" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -9215,7 +9341,10 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M2"/>
+      <c r="P2"/>
+    </row>
     <row r="3" spans="1:19" s="10" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>74</v>
@@ -9229,14 +9358,26 @@
       <c r="D3" s="47" t="s">
         <v>69</v>
       </c>
+      <c r="M3" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="O3" s="99" t="s">
+        <v>147</v>
+      </c>
+      <c r="P3" s="99" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4"/>
@@ -9254,6 +9395,18 @@
       </c>
       <c r="D5" s="42" t="s">
         <v>43</v>
+      </c>
+      <c r="M5" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="O5" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="P5" s="100" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -9322,6 +9475,15 @@
       <c r="M10" s="40" t="s">
         <v>86</v>
       </c>
+      <c r="N10" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="O10" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="P10" s="99" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -9372,8 +9534,17 @@
       <c r="L12" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="101" t="s">
         <v>36</v>
+      </c>
+      <c r="N12" s="101" t="s">
+        <v>152</v>
+      </c>
+      <c r="O12" s="101" t="s">
+        <v>153</v>
+      </c>
+      <c r="P12" s="101" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -9381,6 +9552,9 @@
         <v>22</v>
       </c>
       <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
@@ -9402,6 +9576,9 @@
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -9438,7 +9615,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="81" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>

</xml_diff>

<commit_message>
fix templates for extra
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionBook/Masters-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionBook/Masters-A4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979987EC-A17A-4EE6-BF90-D5875C546F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AE7163-D14F-4483-B3E6-245311F0D8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="555" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="33" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="158">
   <si>
     <t>M/F</t>
   </si>
@@ -116,9 +116,6 @@
     <t>${l.total}</t>
   </si>
   <si>
-    <t>${l.rank}</t>
-  </si>
-  <si>
     <t>&lt;/jx:forEach&gt;</t>
   </si>
   <si>
@@ -516,6 +513,18 @@
   </si>
   <si>
     <t>$[countif(j12:j12,3)]</t>
+  </si>
+  <si>
+    <t>${l.snatchRank &lt; 0 ? t.get("Results.Extra/Invited") : l.snatchRank}</t>
+  </si>
+  <si>
+    <t>${l.cleanJerkRank &lt; 0 ? t.get("Results.Extra/Invited") : l.cleanJerkRank}</t>
+  </si>
+  <si>
+    <t>${l.totalRank &lt; 0 ? t.get("Results.Extra/Invited") : l.totalRank}</t>
+  </si>
+  <si>
+    <t>${l.qAgeRank &lt; 0 ? t.get("Results.Extra/Invited") : l.qAgeRank}</t>
   </si>
 </sst>
 </file>
@@ -531,7 +540,7 @@
     <numFmt numFmtId="169" formatCode="0;&quot;&quot;"/>
     <numFmt numFmtId="170" formatCode="0;&quot;&quot;;\-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -648,6 +657,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1157,7 +1172,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1210,10 +1225,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1435,6 +1446,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1462,22 +1490,27 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1503,27 +1536,12 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2060,69 +2078,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="102" t="s">
+      <c r="A1" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53" t="s">
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="51" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53" t="s">
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="103" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="53"/>
+      <c r="B3" s="102" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="52"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="H4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="H4" s="52"/>
     </row>
     <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
+      <c r="A5" s="59"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="N6"/>
@@ -2133,167 +2151,167 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="50" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
       <c r="I8" t="s">
-        <v>106</v>
-      </c>
-      <c r="J8" s="55"/>
-      <c r="L8" s="57"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="56"/>
-      <c r="Q8" s="55"/>
+        <v>105</v>
+      </c>
+      <c r="J8" s="54"/>
+      <c r="L8" s="56"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="54"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="51"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="50"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
       <c r="K9"/>
-      <c r="L9" s="55"/>
-      <c r="N9" s="57"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="55"/>
-    </row>
-    <row r="10" spans="1:19" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="51" t="s">
+      <c r="L9" s="54"/>
+      <c r="N9" s="56"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="54"/>
+    </row>
+    <row r="10" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="H10" s="53" t="s">
+      <c r="D10" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="H10" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="L10" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="M10" s="51" t="s">
+      <c r="I10" s="50" t="s">
         <v>101</v>
       </c>
+      <c r="L10" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="M10" s="50" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C11" s="53" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="51" t="s">
+      <c r="C11" s="52" t="s">
         <v>99</v>
       </c>
+      <c r="D11" s="50" t="s">
+        <v>98</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="H11" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="51" t="s">
+      <c r="H11" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="I11" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="50"/>
       <c r="K11" s="1"/>
-      <c r="M11" s="51" t="s">
-        <v>96</v>
+      <c r="M11" s="50" t="s">
+        <v>95</v>
       </c>
       <c r="N11" s="1"/>
       <c r="P11"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="52"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="51"/>
       <c r="S11"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C12" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="51" t="s">
+      <c r="C12" s="52" t="s">
         <v>94</v>
       </c>
+      <c r="D12" s="50" t="s">
+        <v>93</v>
+      </c>
       <c r="E12" s="1"/>
-      <c r="H12" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="I12" s="51" t="s">
+      <c r="H12" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="51"/>
+      <c r="I12" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="50"/>
       <c r="K12" s="1"/>
-      <c r="M12" s="51" t="s">
-        <v>91</v>
+      <c r="M12" s="50" t="s">
+        <v>90</v>
       </c>
       <c r="N12" s="1"/>
-      <c r="O12" s="51"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="52"/>
+      <c r="O12" s="50"/>
+      <c r="Q12" s="53"/>
+      <c r="R12" s="51"/>
       <c r="S12"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C13" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="52" t="s">
+      <c r="C13" s="52" t="s">
         <v>89</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="M13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N13"/>
       <c r="S13"/>
     </row>
     <row r="14" spans="1:19" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
     </row>
     <row r="15" spans="1:19" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
+      <c r="E15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N16"/>
       <c r="O16"/>
@@ -3778,188 +3796,188 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:24" s="67" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:24" s="68" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="J2" s="68"/>
+    </row>
+    <row r="3" spans="1:24" s="67" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="70"/>
+      <c r="V3" s="70"/>
+    </row>
+    <row r="4" spans="1:24" s="80" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A4" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="69"/>
-    </row>
-    <row r="3" spans="1:24" s="68" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="71"/>
-    </row>
-    <row r="4" spans="1:24" s="81" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A4" s="72" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="75" t="s">
+      <c r="E4" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="F4" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="77" t="s">
+      <c r="H4" s="77"/>
+      <c r="I4" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="78"/>
-      <c r="I4" s="75" t="s">
+      <c r="J4" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="J4" s="72" t="s">
+      <c r="K4" s="78"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="72"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="R4" s="72"/>
+      <c r="S4" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="K4" s="79"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="O4" s="73"/>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="R4" s="73"/>
-      <c r="S4" s="72" t="s">
+      <c r="T4" s="78"/>
+      <c r="U4" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="72" t="s">
+      <c r="V4" s="79"/>
+      <c r="X4" s="73"/>
+    </row>
+    <row r="5" spans="1:24" s="85" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="V4" s="80"/>
-      <c r="X4" s="74"/>
-    </row>
-    <row r="5" spans="1:24" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82" t="s">
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="84"/>
+      <c r="M5" s="84"/>
+    </row>
+    <row r="6" spans="1:24" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="85"/>
-      <c r="M5" s="85"/>
-    </row>
-    <row r="6" spans="1:24" s="95" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="87" t="s">
+      <c r="B6" s="87"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="90" t="s">
+      <c r="E6" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="F6" s="86" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="G6" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="88"/>
+      <c r="I6" s="92" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="91" t="s">
+      <c r="J6" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="H6" s="89"/>
-      <c r="I6" s="93" t="s">
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="J6" s="91" t="s">
-        <v>140</v>
-      </c>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="91" t="s">
+      <c r="O6" s="87"/>
+      <c r="P6" s="88"/>
+      <c r="Q6" s="86" t="s">
         <v>133</v>
       </c>
-      <c r="O6" s="88"/>
-      <c r="P6" s="89"/>
-      <c r="Q6" s="87" t="s">
+      <c r="R6" s="87"/>
+      <c r="S6" s="91" t="s">
         <v>134</v>
       </c>
-      <c r="R6" s="88"/>
-      <c r="S6" s="92" t="s">
+      <c r="T6" s="87"/>
+      <c r="U6" s="93" t="s">
         <v>135</v>
       </c>
-      <c r="T6" s="88"/>
-      <c r="U6" s="94" t="s">
+      <c r="V6" s="88"/>
+      <c r="X6" s="88"/>
+    </row>
+    <row r="7" spans="1:24" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="82"/>
+      <c r="W7"/>
+    </row>
+    <row r="8" spans="1:24" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="94" t="s">
         <v>136</v>
       </c>
-      <c r="V6" s="89"/>
-      <c r="X6" s="89"/>
-    </row>
-    <row r="7" spans="1:24" s="95" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="95" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="97"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="83"/>
-      <c r="W7"/>
-    </row>
-    <row r="8" spans="1:24" s="95" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="95" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="97"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="83"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="95"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="82"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D5">
@@ -4010,10 +4028,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
         <v>114</v>
-      </c>
-      <c r="B1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5643,7 +5661,7 @@
   <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5672,59 +5690,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="104" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="104" t="s">
+      <c r="A1" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="B1" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="112" t="s">
+      <c r="C1" s="110" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="112" t="s">
+      <c r="G1" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="112" t="s">
+      <c r="H1" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="112" t="s">
+      <c r="I1" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="114" t="s">
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="115" t="s">
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="110" t="s">
-        <v>78</v>
-      </c>
-      <c r="T1" s="110"/>
+      <c r="T1" s="114"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="105"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="38">
+      <c r="A2" s="109"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="37">
         <v>1</v>
       </c>
       <c r="J2" s="12">
@@ -5733,11 +5751,11 @@
       <c r="K2" s="12">
         <v>3</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="35" t="s">
         <v>79</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>80</v>
       </c>
       <c r="N2" s="12">
         <v>1</v>
@@ -5748,22 +5766,22 @@
       <c r="P2" s="12">
         <v>3</v>
       </c>
-      <c r="Q2" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="R2" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>80</v>
+      <c r="Q2" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -5782,68 +5800,68 @@
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" s="5" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="29" t="s">
+      <c r="E4" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
+      <c r="H4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="127" t="s">
+        <v>154</v>
+      </c>
+      <c r="N4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="24" t="s">
+      <c r="R4" s="127" t="s">
+        <v>155</v>
+      </c>
+      <c r="S4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="23" t="s">
-        <v>21</v>
+      <c r="T4" s="128" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -5881,11 +5899,11 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
-      <c r="R12" s="111"/>
+      <c r="R12" s="103"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
-      <c r="R13" s="111"/>
+      <c r="R13" s="103"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
@@ -6163,6 +6181,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="R12:R13"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
@@ -6170,11 +6193,6 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:R1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5">
     <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
@@ -6204,8 +6222,8 @@
   </sheetPr>
   <dimension ref="A1:W102"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6231,62 +6249,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="117" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="117" t="s">
+      <c r="A1" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="B1" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="112" t="s">
+      <c r="C1" s="124" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="G1" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="122" t="s">
+      <c r="H1" s="116" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="123" t="s">
+      <c r="I1" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="125" t="s">
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125" t="s">
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="126" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="114" t="s">
-        <v>142</v>
-      </c>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
+      <c r="R1" s="106" t="s">
+        <v>141</v>
+      </c>
+      <c r="S1" s="106"/>
+      <c r="T1" s="106"/>
       <c r="V1"/>
       <c r="W1"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="124"/>
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="12">
         <v>1</v>
       </c>
@@ -6296,7 +6314,7 @@
       <c r="K2" s="12">
         <v>3</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="12">
@@ -6308,23 +6326,23 @@
       <c r="O2" s="12">
         <v>3</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="S2" s="39" t="s">
+      <c r="Q2" s="120"/>
+      <c r="R2" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="T2" s="50" t="s">
-        <v>80</v>
+      <c r="S2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="T2" s="49" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -6346,63 +6364,63 @@
       <c r="W3"/>
     </row>
     <row r="4" spans="1:23" s="5" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="61" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="26" t="s">
+      <c r="M4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="N4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="64" t="s">
+      <c r="R4" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="S4" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="S4" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="T4" s="66" t="s">
-        <v>48</v>
+      <c r="T4" s="65" t="s">
+        <v>157</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>2</v>
@@ -6410,7 +6428,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -6446,11 +6464,11 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
-      <c r="R10" s="111"/>
+      <c r="R10" s="103"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
-      <c r="R11" s="111"/>
+      <c r="R11" s="103"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
@@ -6728,6 +6746,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="R10:R11"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
@@ -6735,12 +6759,6 @@
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C4">
     <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
@@ -6770,8 +6788,8 @@
   </sheetPr>
   <dimension ref="A1:W102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6797,62 +6815,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="117" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="117" t="s">
+      <c r="A1" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="B1" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="112" t="s">
+      <c r="C1" s="124" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="G1" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="122" t="s">
+      <c r="H1" s="116" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="123" t="s">
+      <c r="I1" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="125" t="s">
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125" t="s">
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="126" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="114" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
+      <c r="R1" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="106"/>
+      <c r="T1" s="106"/>
       <c r="V1"/>
       <c r="W1"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="124"/>
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="12">
         <v>1</v>
       </c>
@@ -6862,7 +6880,7 @@
       <c r="K2" s="12">
         <v>3</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="12">
@@ -6874,23 +6892,23 @@
       <c r="O2" s="12">
         <v>3</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="S2" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" s="50" t="s">
+      <c r="Q2" s="120"/>
+      <c r="R2" s="48" t="s">
         <v>80</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" s="49" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -6912,63 +6930,63 @@
       <c r="W3"/>
     </row>
     <row r="4" spans="1:23" s="5" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="61" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="63" t="s">
+      <c r="I4" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="65" t="s">
         <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="66" t="s">
-        <v>48</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>2</v>
@@ -6976,7 +6994,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -7012,11 +7030,11 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
-      <c r="R10" s="111"/>
+      <c r="R10" s="103"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
-      <c r="R11" s="111"/>
+      <c r="R11" s="103"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
@@ -7294,6 +7312,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="R10:R11"/>
     <mergeCell ref="G1:G2"/>
@@ -7302,11 +7325,6 @@
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C4">
     <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
@@ -7337,7 +7355,7 @@
   <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7365,59 +7383,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="104" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="104" t="s">
+      <c r="A1" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="B1" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="112" t="s">
+      <c r="C1" s="110" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="112" t="s">
+      <c r="G1" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="112" t="s">
+      <c r="H1" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="112" t="s">
+      <c r="I1" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="114" t="s">
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="115" t="s">
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="110" t="s">
-        <v>78</v>
-      </c>
-      <c r="T1" s="110"/>
+      <c r="T1" s="114"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="105"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="38">
+      <c r="A2" s="109"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="37">
         <v>1</v>
       </c>
       <c r="J2" s="12">
@@ -7426,11 +7444,11 @@
       <c r="K2" s="12">
         <v>3</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="35" t="s">
         <v>79</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>80</v>
       </c>
       <c r="N2" s="12">
         <v>1</v>
@@ -7441,22 +7459,22 @@
       <c r="P2" s="12">
         <v>3</v>
       </c>
-      <c r="Q2" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="R2" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>80</v>
+      <c r="Q2" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -7475,68 +7493,68 @@
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" s="5" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="29" t="s">
+      <c r="E4" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
+      <c r="H4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="127" t="s">
+        <v>154</v>
+      </c>
+      <c r="N4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="24" t="s">
+      <c r="R4" s="127" t="s">
+        <v>155</v>
+      </c>
+      <c r="S4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="23" t="s">
-        <v>21</v>
+      <c r="T4" s="128" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -7575,11 +7593,11 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
-      <c r="R12" s="111"/>
+      <c r="R12" s="103"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
-      <c r="R13" s="111"/>
+      <c r="R13" s="103"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
@@ -7857,6 +7875,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="N1:R1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="R12:R13"/>
     <mergeCell ref="E1:E2"/>
@@ -7864,11 +7887,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:M1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5">
     <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
@@ -7899,7 +7917,7 @@
   <dimension ref="A1:W97"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7924,62 +7942,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="117" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="117" t="s">
+      <c r="A1" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="B1" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="112" t="s">
+      <c r="C1" s="124" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="G1" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="122" t="s">
+      <c r="H1" s="116" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="123" t="s">
+      <c r="I1" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="125" t="s">
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125" t="s">
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="126" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="114" t="s">
-        <v>142</v>
-      </c>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
+      <c r="R1" s="106" t="s">
+        <v>141</v>
+      </c>
+      <c r="S1" s="106"/>
+      <c r="T1" s="106"/>
       <c r="V1"/>
       <c r="W1"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="124"/>
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="12">
         <v>1</v>
       </c>
@@ -7989,7 +8007,7 @@
       <c r="K2" s="12">
         <v>3</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="12">
@@ -8001,23 +8019,23 @@
       <c r="O2" s="12">
         <v>3</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="S2" s="39" t="s">
+      <c r="Q2" s="120"/>
+      <c r="R2" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="T2" s="50" t="s">
-        <v>80</v>
+      <c r="S2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="T2" s="49" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -8039,63 +8057,63 @@
       <c r="W3"/>
     </row>
     <row r="4" spans="1:23" s="5" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="61" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="26" t="s">
+      <c r="M4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="N4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="64" t="s">
+      <c r="R4" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="S4" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="S4" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="T4" s="66" t="s">
-        <v>48</v>
+      <c r="T4" s="65" t="s">
+        <v>157</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>2</v>
@@ -8103,7 +8121,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -8138,11 +8156,11 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
-      <c r="R10" s="111"/>
+      <c r="R10" s="103"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
-      <c r="R11" s="111"/>
+      <c r="R11" s="103"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
@@ -8405,6 +8423,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="R10:R11"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
@@ -8412,12 +8436,6 @@
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C4">
     <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
@@ -8473,62 +8491,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="117" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="117" t="s">
+      <c r="A1" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="B1" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="112" t="s">
+      <c r="C1" s="124" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="G1" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="122" t="s">
+      <c r="H1" s="116" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="123" t="s">
+      <c r="I1" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="125" t="s">
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125" t="s">
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="126" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="114" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
+      <c r="R1" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="106"/>
+      <c r="T1" s="106"/>
       <c r="V1"/>
       <c r="W1"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="124"/>
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="12">
         <v>1</v>
       </c>
@@ -8538,7 +8556,7 @@
       <c r="K2" s="12">
         <v>3</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="12">
@@ -8550,23 +8568,23 @@
       <c r="O2" s="12">
         <v>3</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="S2" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" s="50" t="s">
+      <c r="Q2" s="120"/>
+      <c r="R2" s="48" t="s">
         <v>80</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" s="49" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -8588,63 +8606,63 @@
       <c r="W3"/>
     </row>
     <row r="4" spans="1:23" s="5" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="61" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="63" t="s">
+      <c r="I4" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="66" t="s">
         <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="67" t="s">
-        <v>48</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>2</v>
@@ -8652,7 +8670,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -8953,6 +8971,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="F1:F2"/>
@@ -8960,11 +8983,6 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:P1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C4">
     <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
@@ -9016,7 +9034,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -9026,34 +9044,34 @@
       <c r="P2"/>
     </row>
     <row r="3" spans="1:19" s="10" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" s="45" t="s">
+      <c r="A3" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="O3" s="98" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="99" t="s">
+      <c r="P3" s="98" t="s">
         <v>147</v>
-      </c>
-      <c r="P3" s="99" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="20"/>
       <c r="M4"/>
@@ -9065,34 +9083,34 @@
       <c r="S4"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="42" t="s">
+      <c r="A5" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="O5" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="O5" s="42" t="s">
+      <c r="P5" s="99" t="s">
         <v>150</v>
-      </c>
-      <c r="P5" s="100" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M6"/>
       <c r="N6"/>
@@ -9110,65 +9128,65 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:19" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="41" t="s">
+      <c r="A10" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="41" t="s">
+      <c r="C10" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="41" t="s">
-        <v>74</v>
-      </c>
       <c r="G10" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="L10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="M10" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="M10" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="N10" s="40" t="s">
+      <c r="N10" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="O10" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="O10" s="40" t="s">
+      <c r="P10" s="98" t="s">
         <v>147</v>
-      </c>
-      <c r="P10" s="99" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M11"/>
       <c r="N11"/>
@@ -9189,48 +9207,48 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="15" t="s">
-        <v>25</v>
-      </c>
       <c r="J12" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="100" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" s="100" t="s">
+        <v>151</v>
+      </c>
+      <c r="O12" s="100" t="s">
         <v>152</v>
       </c>
-      <c r="O12" s="101" t="s">
+      <c r="P12" s="100" t="s">
         <v>153</v>
-      </c>
-      <c r="P12" s="101" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M13"/>
       <c r="N13"/>
@@ -9263,27 +9281,27 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -9336,7 +9354,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -9346,34 +9364,34 @@
       <c r="P2"/>
     </row>
     <row r="3" spans="1:19" s="10" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" s="45" t="s">
+      <c r="A3" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="O3" s="98" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="99" t="s">
+      <c r="P3" s="98" t="s">
         <v>147</v>
-      </c>
-      <c r="P3" s="99" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M4"/>
       <c r="N4" s="20"/>
@@ -9384,34 +9402,34 @@
       <c r="S4"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="42" t="s">
+      <c r="A5" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="42" t="s">
+      <c r="M5" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="O5" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="O5" s="42" t="s">
+      <c r="P5" s="99" t="s">
         <v>150</v>
-      </c>
-      <c r="P5" s="100" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M6"/>
       <c r="N6"/>
@@ -9429,65 +9447,65 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:19" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="41" t="s">
+      <c r="A10" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="41" t="s">
+      <c r="C10" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="41" t="s">
-        <v>74</v>
-      </c>
       <c r="G10" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="L10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="M10" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="M10" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="N10" s="40" t="s">
+      <c r="N10" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="O10" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="O10" s="40" t="s">
+      <c r="P10" s="98" t="s">
         <v>147</v>
-      </c>
-      <c r="P10" s="99" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M11"/>
       <c r="N11"/>
@@ -9508,48 +9526,48 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="15" t="s">
-        <v>25</v>
-      </c>
       <c r="J12" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="100" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" s="100" t="s">
+        <v>151</v>
+      </c>
+      <c r="O12" s="100" t="s">
         <v>152</v>
       </c>
-      <c r="O12" s="101" t="s">
+      <c r="P12" s="100" t="s">
         <v>153</v>
-      </c>
-      <c r="P12" s="101" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M13"/>
       <c r="N13"/>
@@ -9582,27 +9600,27 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>